<commit_message>
update docs (accounts OK)
</commit_message>
<xml_diff>
--- a/doc/accounts解析.xlsx
+++ b/doc/accounts解析.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\user1\work\workspace\git\bookproject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D34A93-FC8E-4515-B510-8C888BF145DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA620813-5B11-48B3-9466-2D3CED0CE18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="apps.py" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="104">
   <si>
     <r>
       <t>from</t>
@@ -3419,6 +3419,63 @@
   </si>
   <si>
     <t>↑</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>見出し部分（&lt;h1&gt;）などに使うカスタムブロック</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Django のセキュリティ機能。
+クロスサイトリクエストフォージェリ（CSRF）攻撃を防ぐために、POST フォームには必ず入れる必要があります。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bootstrap のクラスを使って、フォームにパディング・マージン・背景色・枠線・角丸などの装飾を加えてる</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>postリクエストを指定。</t>
+    <rPh sb="10" eb="12">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メインのフォーム部分</t>
+    <rPh sb="8" eb="10">
+      <t>ブブン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ユーザーに対する入力ガイド</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>form.errors にエラーがあれば、表示されます。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>緑色の「アカウント作成」ボタン。
+Bootstrap の btn btn-success クラスで見た目が良く整っています。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>input欄の用意。</t>
+    <rPh sb="5" eb="6">
+      <t>ラン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヨウイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Djangoと接続される。</t>
+    <rPh sb="7" eb="9">
+      <t>セツゾク</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3560,7 +3617,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3577,7 +3634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3605,10 +3662,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -4015,76 +4075,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>4695825</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="テキスト ボックス 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42C5D5FC-3D97-2C84-2EAC-7C6C6741C6DA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13601700" y="8724901"/>
-          <a:ext cx="3267075" cy="704850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFF00"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>パスワード入力も必要だったがどこに保存？</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4231,15 +4221,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
+      <xdr:colOff>514348</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>4848224</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2400299</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4254,14 +4244,17 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1200149" y="7753350"/>
-          <a:ext cx="4333875" cy="1409700"/>
+          <a:off x="1200148" y="10467975"/>
+          <a:ext cx="9448801" cy="10210800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="FFFF00"/>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
           <a:solidFill>
@@ -4335,6 +4328,1113 @@
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
             <a:t>に指定しているから？</a:t>
           </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>↓</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>はい、まさにその通りです！🌟</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>form </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>という変数がテンプレート内で使える理由は、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" b="1"/>
+            <a:t>CreateView</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>（や他のフォーム系</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" b="1"/>
+            <a:t>CBV</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>）がテンプレートに </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" b="1"/>
+            <a:t>form </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>というコンテキスト変数を自動的に渡してくれるから</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>です。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>以下に詳しく仕組みを解説しますね。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>✅ 簡潔に言うと：</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>class SignupView(CreateView):</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>    form_class = SignupForm</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>    ...</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ja-JP"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>このように </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>CreateView </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>を使っていると、テンプレート内では自動的に以下のような変数が使えるようになります：</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>form ← </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>フォームオブジェクト（</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>SignupForm()</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>のインスタンス）</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>object</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>（編集系ビューの場合のみ）</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>その他、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>CBV</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>ごとに必要な変数</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>🔍 なぜ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" b="1"/>
+            <a:t>form </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>が使えるの？</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>Django </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>の </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>CreateView </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>は、内部でテンプレートに渡す「コンテキスト（辞書のようなもの）」を自動で作成しています：</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>def get_context_data(self, **kwargs):</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>    context = super().get_context_data(**kwargs)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>    context['form'] = self.get_form()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>    return context</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ja-JP"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>このようにして </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>form </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>がテンプレートに渡されているのです。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>🧪 テンプレートではどう使われる？</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>たとえば以下のように書くと：</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>&lt;form method="post"&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>  {% csrf_token %}</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>  {{ form.as_p }}</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>&lt;/form&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ja-JP"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>この </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>{{ form.as_p }} </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>が使えるのは、テンプレートに </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>form </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>が渡されているからです。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>🛠️ 自分でテンプレート変数名を変えたいときは？</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>どうしても </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>form </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>という名前以外にしたい場合は、ビュー側で </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>get_context_data() </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>をオーバーライドすることで変更できます：</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>class SignupView(CreateView):</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>    ...</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ja-JP"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>    def get_context_data(self, **kwargs):</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>        context = super().get_context_data(**kwargs)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>        context['my_form'] = context.pop('form')  # </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>名前を変更</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>        </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>return context</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ja-JP"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>テンプレートでは </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>{{ my_form.as_p }} </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>のように使えます。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>🎓 まとめ</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>役割 内容 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>form </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>変数 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>CreateView, UpdateView, FormView </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>などで自動で使える 自動連携の理由 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>get_context_data() </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>によってテンプレートに </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>form </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>が渡される 必要な設定 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>form_class or model </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>を </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>CreateView </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>に指定しておく 本当にいい質問でした👏</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>「なぜそうなるのか」を一歩深掘りして考えられているのが素晴らしいです！</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>さらに学びを進めたいときは、たとえば </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>form_valid() </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>の使い方や、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>form.save() </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>のカスタマイズもおすすめですよ。興味ありますか？</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>148877</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1155805</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>530679</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="テキスト ボックス 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13DE4D5E-4195-E4D5-F229-E7815EE154D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11883677" y="4251430"/>
+          <a:ext cx="11354602" cy="8121545"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>とても良い視点ですね！✨</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>&lt;input name="username"&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>が </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>Django </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>のフォームと「接続される理由」は、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" b="1"/>
+            <a:t>Django </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>の </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" b="1"/>
+            <a:t>Form / ModelForm </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>が内部的にそのフィールド名をキーとして処理しているから</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>です。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>では、順を追って丁寧に解説します。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>🔁 フォームのデータ送信の流れ（</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" b="1"/>
+            <a:t>HTML ⇔ Django</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>）</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" b="1"/>
+            <a:t>1. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>フォーム送信時の仕組み（ブラウザ側）</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>&lt;input name="username" ...&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>フォームが送信されると、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>POST </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>データの中に </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>username=xxxxx </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>のようなデータが入ります。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>つまり、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>request.POST </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>の中に </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>'username': '</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>フォームに入力された値</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>' </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>が入るということです。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" b="1"/>
+            <a:t>2. Django </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>側のフォーム（</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" b="1"/>
+            <a:t>UserCreationForm</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>）</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>あなたが使っている </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>SignupForm </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>は、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>Django </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>の </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>UserCreationForm </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>を継承しています：</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>class SignupForm(UserCreationForm):</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>    class Meta:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>        model = User</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>        fields = ("username",)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ja-JP"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ja-JP"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>は、内部で </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>username, password1, password2 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>というフィールドを定義しています。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>Django </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>はこのフィールド名を元に、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>request.POST </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>の中身と自動で対応づけてくれます。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>✅ つまりこういうこと</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>HTML</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>側で </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>&lt;input name="username"&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>と書くと、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>request.POST["username"] </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>にデータが入る。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>Django</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>の</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>Form</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>は</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>username</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>というフィールドを持っている。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>Django</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>のフォーム処理は、その名前で一致するキーを</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>request.POST</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>から探し、自動的にマッピングしてくれる。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>💡 少し専門的に言うと</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" b="1"/>
+            <a:t>…</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>Django</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>のフォームは、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>name</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>属性と一致するキーを </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>request.POST </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>や </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>request.FILES </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>から探し、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>form.cleaned_data </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>に流し込む。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>これは </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>名前によるバインディング（</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" b="1"/>
+            <a:t>field name binding</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>）</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>と呼ばれる仕組みです。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>🎓 もし名前が違ったら？</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>たとえば </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>HTML </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>側で：</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>&lt;input name="user_name"&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>と書いた場合は、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>form.cleaned_data["username"] </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>には</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>何も渡りません！</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>→ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>user_name </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>というキーは </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>Form </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>側に存在しないので、無視されます。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>🧪 まとめ</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>HTML </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>の </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>name </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>属性 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>Django </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>フォームでのフィールド名 接続される？ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>name="username" username = forms.CharField() </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>✅ 接続される </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>name="user_id" username = forms.CharField() </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>❌ 無視される </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>Django </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>がうまく処理してくれるのは、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
+            <a:t>名前が一致しているからこそ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>。</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>つまり、「</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>Django </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>のフォームと接続される＝フィールド名と </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>name </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>属性が一致しているから」ということです！</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>よく気がつきましたね👏</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>もし「じゃあフォームから動的に名前を出力する方法は？」「自動で </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>name </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>や </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
+            <a:t>id </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
+            <a:t>をレンダリングしてくれる方法は？」なんてことが気になれば、それも大事なステップです。知りたいですか？</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4608,9 +5708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37007A8D-9AFB-467E-8FF9-689D81AA5519}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -4703,7 +5801,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="168.75">
-      <c r="A1" s="11"/>
+      <c r="A1" s="13" t="s">
+        <v>61</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4869,7 +5969,9 @@
       <c r="C16" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="11"/>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -4882,9 +5984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED561DA-63B9-4703-B6BB-E9FDA0D9CBBF}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -5041,9 +6141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1569785-B1B5-418C-A16A-E1630FD51E20}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -5219,11 +6317,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA281EBE-CD95-4452-A303-0204600DC801}">
-  <dimension ref="B1:D30"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -5231,7 +6327,10 @@
     <col min="3" max="3" width="45.75" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="1:4">
+      <c r="A1" s="13" t="s">
+        <v>61</v>
+      </c>
       <c r="B1" s="4" t="s">
         <v>32</v>
       </c>
@@ -5242,7 +6341,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="37.5">
+    <row r="2" spans="1:4" ht="37.5">
       <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
@@ -5253,7 +6352,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="1:4">
       <c r="B3" s="4" t="s">
         <v>34</v>
       </c>
@@ -5264,7 +6363,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="1:4">
       <c r="B4" s="4" t="s">
         <v>35</v>
       </c>
@@ -5275,132 +6374,225 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="1:4">
       <c r="B5" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="2:4">
+      <c r="C5" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="B6" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="2:4">
+      <c r="C6" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="B7" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="2:4">
+      <c r="C7" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="B8" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="2:4">
+      <c r="C8" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="B9" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="2:4">
+      <c r="C9" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="56.25">
       <c r="B10" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="2:4">
+      <c r="C10" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="93.75">
       <c r="B11" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="2:4">
+      <c r="C11" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="B12" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="2:4">
+      <c r="C12" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="B13" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="2:4">
+      <c r="C13" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="B14" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="2:4">
+      <c r="C14" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="B15" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="2:4">
+      <c r="C15" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="B16" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="2:2">
+      <c r="C16" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
       <c r="B17" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="2:2">
+      <c r="C17" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
       <c r="B18" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="2:2">
+      <c r="C18" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
       <c r="B19" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="2:2">
+      <c r="C19" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
       <c r="B20" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="2:2">
+      <c r="C20" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
       <c r="B21" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="2:2">
+      <c r="C21" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
       <c r="B22" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="2:2">
+      <c r="C22" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
       <c r="B23" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="2:2">
+      <c r="C23" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
       <c r="B24" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="2:2">
+      <c r="C24" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
       <c r="B25" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" ht="45" customHeight="1">
-      <c r="B26" s="12" t="s">
+      <c r="C25" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="45" customHeight="1">
+      <c r="B26" s="11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="27" spans="2:2">
+      <c r="C26" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
       <c r="B27" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="2:2">
+      <c r="C27" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="75">
       <c r="B28" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="2:2">
+      <c r="C28" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
       <c r="B29" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="2:2">
+    <row r="30" spans="2:3">
       <c r="B30" s="4" t="s">
         <v>57</v>
       </c>

</xml_diff>